<commit_message>
New API Tests Uploaded
</commit_message>
<xml_diff>
--- a/DataNE.xlsx
+++ b/DataNE.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="16500" yWindow="12300" windowWidth="19960" windowHeight="9580" tabRatio="500"/>
+    <workbookView xWindow="14120" yWindow="11860" windowWidth="18220" windowHeight="8460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Login Info" sheetId="1" r:id="rId1"/>
@@ -473,7 +473,7 @@
   <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Updated Test Suite File
</commit_message>
<xml_diff>
--- a/DataNE.xlsx
+++ b/DataNE.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="820" windowWidth="29860" windowHeight="12520" tabRatio="500"/>
+    <workbookView xWindow="160" yWindow="620" windowWidth="29860" windowHeight="12520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Login Info" sheetId="1" r:id="rId1"/>
@@ -561,7 +561,7 @@
         <v>3</v>
       </c>
       <c r="D2" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2" s="2">
         <v>1</v>

</xml_diff>